<commit_message>
suite et correction acp
</commit_message>
<xml_diff>
--- a/BI Charlier/Regression linéaire/Suite/ACP/temperaturesEurope.xlsx
+++ b/BI Charlier/Regression linéaire/Suite/ACP/temperaturesEurope.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17426"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Damien Jacques\Documents\Business-Intelligence\BI Charlier\Regression linéaire\Suite\ACP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Wrkfldr\Business-Intelligence\BI Charlier\Regression linéaire\Suite\ACP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Amsterdam</t>
   </si>
@@ -144,12 +144,15 @@
   </si>
   <si>
     <t>Zurich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moyenne </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -521,13 +524,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
@@ -1714,6 +1717,59 @@
       </c>
       <c r="M29" s="1">
         <v>0.3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31">
+        <f>AVERAGE(B2:B29)</f>
+        <v>1.9321428571428574</v>
+      </c>
+      <c r="C31">
+        <f t="shared" ref="C31:M31" si="0">AVERAGE(C2:C29)</f>
+        <v>2.8321428571428564</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>5.8571428571428594</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>9.7571428571428562</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>14.27142857142857</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>17.8</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="0"/>
+        <v>20.010714285714279</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="0"/>
+        <v>19.410714285714288</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="0"/>
+        <v>16.142857142857142</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="0"/>
+        <v>11.546428571428569</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="0"/>
+        <v>6.5857142857142863</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="0"/>
+        <v>3.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>